<commit_message>
Doku V2 fin Stand 27.03.
</commit_message>
<xml_diff>
--- a/Dokumentation/Projektplan/Projektplan_Lendl.xlsx
+++ b/Dokumentation/Projektplan/Projektplan_Lendl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{77EF9C38-9E73-41B5-8BDB-AC5DAC882043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{203ACCF7-770C-4DFA-807B-333499E53FEF}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{77EF9C38-9E73-41B5-8BDB-AC5DAC882043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35B11161-8BDB-40DF-B27E-FC33EA568A50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,7 +571,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ16" sqref="AZ16"/>
+      <selection pane="bottomRight" activeCell="AV30" sqref="AV30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <f t="shared" si="7"/>
         <v>13</v>
@@ -1626,7 +1626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f t="shared" si="7"/>
         <v>14</v>
@@ -1638,7 +1638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f t="shared" si="7"/>
         <v>15</v>
@@ -1649,7 +1649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f t="shared" si="7"/>
         <v>16</v>
@@ -1661,7 +1661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <f t="shared" si="7"/>
         <v>17</v>
@@ -1672,7 +1672,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <f t="shared" si="7"/>
         <v>18</v>
@@ -1688,7 +1688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <f t="shared" si="7"/>
         <v>19</v>
@@ -1700,7 +1700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <f t="shared" si="7"/>
         <v>20</v>
@@ -1710,7 +1710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <f t="shared" si="7"/>
         <v>21</v>
@@ -1722,7 +1722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <f t="shared" si="7"/>
         <v>22</v>
@@ -1733,7 +1733,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <f t="shared" si="7"/>
         <v>23</v>
@@ -1744,7 +1744,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <f t="shared" si="7"/>
         <v>24</v>
@@ -1761,11 +1761,13 @@
       <c r="AR28" s="10"/>
       <c r="AS28" s="10"/>
       <c r="AT28" s="10"/>
-      <c r="AU28" t="s">
+      <c r="AU28" s="10"/>
+      <c r="AV28" s="10"/>
+      <c r="AW28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <f t="shared" si="7"/>
         <v>25</v>
@@ -1776,23 +1778,25 @@
       <c r="AR29" s="10"/>
       <c r="AS29" s="10"/>
       <c r="AT29" s="10"/>
-      <c r="AU29" t="s">
+      <c r="AU29" s="10"/>
+      <c r="AV29" s="10"/>
+      <c r="AW29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <f t="shared" ref="A30:A39" si="8">ROW()-4</f>
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <f t="shared" si="8"/>
         <v>28</v>

</xml_diff>